<commit_message>
My files with analysis
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -11,16 +11,16 @@
     <sheet name="NM" sheetId="2" r:id="rId2"/>
     <sheet name="AL" sheetId="4" r:id="rId3"/>
     <sheet name="2 computers comparison" sheetId="5" r:id="rId4"/>
-    <sheet name="Latest" sheetId="6" r:id="rId5"/>
+    <sheet name="Latest Apr 20" sheetId="8" r:id="rId5"/>
     <sheet name="Grammars" sheetId="7" r:id="rId6"/>
+    <sheet name="Application PL" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="31">
   <si>
     <t xml:space="preserve">BSTinsert </t>
   </si>
@@ -227,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -481,11 +481,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -651,6 +696,77 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,20 +782,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2124,15 +2240,15 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2443,15 +2559,15 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="79" t="s">
+      <c r="I9" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="107"/>
+      <c r="O9" s="107"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -2754,15 +2870,15 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="79" t="s">
+      <c r="I16" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="80"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
     </row>
     <row r="17" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -3093,16 +3209,16 @@
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="81" t="s">
+      <c r="J23" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="83"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="109"/>
+      <c r="N23" s="109"/>
+      <c r="O23" s="109"/>
+      <c r="P23" s="109"/>
+      <c r="Q23" s="110"/>
     </row>
     <row r="24" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -3441,15 +3557,15 @@
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="81" t="s">
+      <c r="I30" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="82"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="82"/>
-      <c r="O30" s="82"/>
+      <c r="J30" s="109"/>
+      <c r="K30" s="109"/>
+      <c r="L30" s="109"/>
+      <c r="M30" s="109"/>
+      <c r="N30" s="109"/>
+      <c r="O30" s="109"/>
     </row>
     <row r="31" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -3780,15 +3896,15 @@
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="84" t="s">
+      <c r="I37" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="85"/>
-      <c r="K37" s="85"/>
-      <c r="L37" s="85"/>
-      <c r="M37" s="85"/>
-      <c r="N37" s="85"/>
-      <c r="O37" s="85"/>
+      <c r="J37" s="103"/>
+      <c r="K37" s="103"/>
+      <c r="L37" s="103"/>
+      <c r="M37" s="103"/>
+      <c r="N37" s="103"/>
+      <c r="O37" s="103"/>
     </row>
     <row r="38" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -4291,15 +4407,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6330,8 +6446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6343,26 +6459,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="76" t="s">
@@ -8223,1133 +8339,2128 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="M2" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27">
-        <v>1027.271</v>
-      </c>
-      <c r="C3" s="27">
-        <v>24.771920000000001</v>
-      </c>
-      <c r="D3" s="27">
-        <v>29.69773</v>
-      </c>
-      <c r="E3" s="27">
-        <v>6.1968240000000003</v>
-      </c>
-      <c r="F3" s="87">
-        <v>3.5830000000000002</v>
-      </c>
-      <c r="H3" s="27">
-        <v>5.0948310000000001</v>
-      </c>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="78">
+        <v>702.12300000000005</v>
+      </c>
+      <c r="C3" s="78">
+        <v>10.99503</v>
+      </c>
+      <c r="D3" s="78">
+        <v>2.5879310000000002</v>
+      </c>
+      <c r="E3" s="78">
+        <v>20.91412</v>
+      </c>
+      <c r="F3" s="78">
+        <v>3.6522019999999999</v>
+      </c>
+      <c r="G3" s="90">
+        <v>2.1619999999999999</v>
+      </c>
+      <c r="J3" s="112">
+        <v>1190.4490000000001</v>
+      </c>
+      <c r="K3" s="78">
+        <v>51.387070000000001</v>
+      </c>
+      <c r="L3" s="93">
+        <v>5.4478689999999999</v>
+      </c>
+      <c r="M3" s="78">
+        <v>34.058450000000001</v>
+      </c>
+      <c r="N3" s="78">
+        <v>13.902839999999999</v>
+      </c>
+      <c r="O3" s="79">
+        <v>10.773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3">
-        <v>30344</v>
-      </c>
-      <c r="C4" s="3">
-        <v>117080</v>
-      </c>
-      <c r="D4" s="3">
-        <v>54476</v>
-      </c>
-      <c r="E4" s="3">
-        <v>87420</v>
-      </c>
-      <c r="F4" s="54">
-        <v>14116</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="5">
+        <v>30224</v>
+      </c>
+      <c r="C4" s="5">
+        <v>116836</v>
+      </c>
+      <c r="D4" s="91">
+        <v>1956</v>
+      </c>
+      <c r="E4" s="5">
+        <v>54320</v>
+      </c>
+      <c r="F4" s="5">
+        <v>85516</v>
+      </c>
+      <c r="G4" s="13">
+        <v>14016</v>
+      </c>
+      <c r="J4" s="12">
+        <v>30692</v>
+      </c>
+      <c r="K4" s="5">
+        <v>117144</v>
+      </c>
+      <c r="L4" s="91">
+        <v>1956</v>
+      </c>
+      <c r="M4" s="5">
+        <v>54528</v>
+      </c>
+      <c r="N4" s="5">
+        <v>87800</v>
+      </c>
+      <c r="O4" s="13">
+        <v>13992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
-        <v>7315</v>
-      </c>
-      <c r="C5" s="3">
-        <v>11090</v>
-      </c>
-      <c r="D5" s="3">
-        <v>8028</v>
-      </c>
-      <c r="E5" s="3">
-        <v>14992</v>
-      </c>
-      <c r="F5" s="54">
-        <v>2120</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="B5" s="5">
+        <v>7320</v>
+      </c>
+      <c r="C5" s="5">
+        <v>11088</v>
+      </c>
+      <c r="D5" s="91">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="E5" s="5">
+        <v>7847</v>
+      </c>
+      <c r="F5" s="5">
+        <v>15231</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2116</v>
+      </c>
+      <c r="J5" s="12">
+        <v>7324</v>
+      </c>
+      <c r="K5" s="5">
+        <v>11089</v>
+      </c>
+      <c r="L5" s="91">
+        <v>140</v>
+      </c>
+      <c r="M5" s="5">
+        <v>7971</v>
+      </c>
+      <c r="N5" s="5">
+        <v>14880</v>
+      </c>
+      <c r="O5" s="13">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3">
-        <v>52</v>
-      </c>
-      <c r="E6" s="3">
-        <v>428</v>
-      </c>
-      <c r="F6" s="54">
+      <c r="B6" s="5">
+        <v>105</v>
+      </c>
+      <c r="C6" s="5">
+        <v>12</v>
+      </c>
+      <c r="D6" s="91">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>273</v>
+      </c>
+      <c r="F6" s="5">
+        <v>645</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <v>399</v>
+      </c>
+      <c r="K6" s="5">
+        <v>431</v>
+      </c>
+      <c r="L6" s="91">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="M6" s="5">
+        <v>300</v>
+      </c>
+      <c r="N6" s="5">
+        <v>2557</v>
+      </c>
+      <c r="O6" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
-        <v>38</v>
-      </c>
-      <c r="C7" s="3">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3">
-        <v>600</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1791</v>
-      </c>
-      <c r="F7" s="54">
+      <c r="B7" s="80">
+        <v>43</v>
+      </c>
+      <c r="C7" s="80">
+        <v>14</v>
+      </c>
+      <c r="D7" s="92">
+        <v>1</v>
+      </c>
+      <c r="E7" s="80">
+        <v>561</v>
+      </c>
+      <c r="F7" s="80">
+        <v>1479</v>
+      </c>
+      <c r="G7" s="81">
+        <v>6</v>
+      </c>
+      <c r="J7" s="16">
+        <v>47</v>
+      </c>
+      <c r="K7" s="80">
+        <v>6</v>
+      </c>
+      <c r="L7" s="92">
+        <v>1</v>
+      </c>
+      <c r="M7" s="80">
+        <v>579</v>
+      </c>
+      <c r="N7" s="80">
+        <v>1184</v>
+      </c>
+      <c r="O7" s="81">
         <v>7</v>
       </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="M9" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27">
-        <v>7.0961080000000001</v>
-      </c>
-      <c r="C10" s="27">
-        <v>46.750059999999998</v>
-      </c>
-      <c r="D10" s="27">
-        <v>5.7325619999999997</v>
-      </c>
-      <c r="E10" s="27">
-        <v>4.3674549999999996</v>
-      </c>
-      <c r="F10" s="87">
-        <v>2.911</v>
-      </c>
-      <c r="H10" s="27">
-        <v>2.3220550000000002</v>
-      </c>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="78">
+        <v>2.9347599999999998</v>
+      </c>
+      <c r="C10" s="78">
+        <v>24.868960000000001</v>
+      </c>
+      <c r="D10" s="93">
+        <v>1.1289739999999999</v>
+      </c>
+      <c r="E10" s="78">
+        <v>3.7337030000000002</v>
+      </c>
+      <c r="F10" s="78">
+        <v>4.005109</v>
+      </c>
+      <c r="G10" s="79">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="J10" s="112">
+        <v>11.07307</v>
+      </c>
+      <c r="K10" s="78">
+        <v>81.849090000000004</v>
+      </c>
+      <c r="L10" s="93">
+        <v>5.4628500000000004</v>
+      </c>
+      <c r="M10" s="78">
+        <v>9.4934270000000005</v>
+      </c>
+      <c r="N10" s="78">
+        <v>19.47522</v>
+      </c>
+      <c r="O10" s="79">
+        <v>6.7110000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>29376</v>
-      </c>
-      <c r="C11" s="3">
-        <v>117216</v>
-      </c>
-      <c r="D11" s="3">
-        <v>55200</v>
-      </c>
-      <c r="E11" s="3">
-        <v>86004</v>
-      </c>
-      <c r="F11" s="54">
-        <v>14040</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="5">
+        <v>29412</v>
+      </c>
+      <c r="C11" s="5">
+        <v>117408</v>
+      </c>
+      <c r="D11" s="91">
+        <v>1956</v>
+      </c>
+      <c r="E11" s="5">
+        <v>54152</v>
+      </c>
+      <c r="F11" s="5">
+        <v>85332</v>
+      </c>
+      <c r="G11" s="13">
+        <v>14124</v>
+      </c>
+      <c r="J11" s="12">
+        <v>29396</v>
+      </c>
+      <c r="K11" s="5">
+        <v>117608</v>
+      </c>
+      <c r="L11" s="93">
+        <v>1972</v>
+      </c>
+      <c r="M11" s="5">
+        <v>55208</v>
+      </c>
+      <c r="N11" s="5">
+        <v>88596</v>
+      </c>
+      <c r="O11" s="13">
+        <v>13956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
+        <v>6943</v>
+      </c>
+      <c r="C12" s="5">
+        <v>11233</v>
+      </c>
+      <c r="D12" s="91">
+        <v>140</v>
+      </c>
+      <c r="E12" s="5">
+        <v>7886</v>
+      </c>
+      <c r="F12" s="5">
+        <v>14574</v>
+      </c>
+      <c r="G12" s="13">
+        <v>2120</v>
+      </c>
+      <c r="J12" s="12">
         <v>6941</v>
       </c>
-      <c r="C12" s="3">
-        <v>11232</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="K12" s="5">
+        <v>11228</v>
+      </c>
+      <c r="L12" s="93">
+        <v>139</v>
+      </c>
+      <c r="M12" s="5">
         <v>8066</v>
       </c>
-      <c r="E12" s="3">
-        <v>15996</v>
-      </c>
-      <c r="F12" s="54">
-        <v>2119</v>
-      </c>
-      <c r="H12" s="3">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="N12" s="5">
+        <v>15036</v>
+      </c>
+      <c r="O12" s="13">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>47</v>
-      </c>
-      <c r="E13" s="3">
-        <v>512</v>
-      </c>
-      <c r="F13" s="54">
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5">
+        <v>18</v>
+      </c>
+      <c r="D13" s="91">
         <v>0</v>
       </c>
-      <c r="H13" s="3">
+      <c r="E13" s="5">
+        <v>400</v>
+      </c>
+      <c r="F13" s="5">
+        <v>637</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <v>259</v>
+      </c>
+      <c r="K13" s="5">
+        <v>262</v>
+      </c>
+      <c r="L13" s="93">
+        <v>8</v>
+      </c>
+      <c r="M13" s="5">
+        <v>316</v>
+      </c>
+      <c r="N13" s="5">
+        <v>2342</v>
+      </c>
+      <c r="O13" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="85">
+        <v>43</v>
+      </c>
+      <c r="C14" s="85">
+        <v>6</v>
+      </c>
+      <c r="D14" s="94">
+        <v>1</v>
+      </c>
+      <c r="E14" s="85">
+        <v>542</v>
+      </c>
+      <c r="F14" s="85">
+        <v>1844</v>
+      </c>
+      <c r="G14" s="86">
+        <v>6</v>
+      </c>
+      <c r="J14" s="16">
+        <v>35</v>
+      </c>
+      <c r="K14" s="80">
+        <v>5</v>
+      </c>
+      <c r="L14" s="113">
+        <v>1</v>
+      </c>
+      <c r="M14" s="80">
+        <v>567</v>
+      </c>
+      <c r="N14" s="80">
+        <v>1370</v>
+      </c>
+      <c r="O14" s="81">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="78">
+        <v>6.0118340000000003</v>
+      </c>
+      <c r="C17" s="78">
+        <v>3.6240809999999999</v>
+      </c>
+      <c r="D17" s="78">
+        <v>2.4544820000000001</v>
+      </c>
+      <c r="E17" s="78">
+        <v>3.8552819999999999</v>
+      </c>
+      <c r="F17" s="78">
+        <v>7.5214040000000004</v>
+      </c>
+      <c r="G17" s="78">
+        <v>1.3340000000000001</v>
+      </c>
+      <c r="H17" s="90">
+        <v>0.40398600000000001</v>
+      </c>
+      <c r="J17" s="112">
+        <v>15.71706</v>
+      </c>
+      <c r="K17" s="78">
+        <v>13.473979999999999</v>
+      </c>
+      <c r="L17" s="78">
+        <v>4.3682129999999999</v>
+      </c>
+      <c r="M17" s="78">
+        <v>7.7112980000000002</v>
+      </c>
+      <c r="N17" s="78">
+        <v>21.256460000000001</v>
+      </c>
+      <c r="O17" s="78">
+        <v>2.5990000000000002</v>
+      </c>
+      <c r="P17" s="90">
+        <v>0.81908099999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5">
+        <v>31092</v>
+      </c>
+      <c r="C18" s="5">
+        <v>114132</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5592</v>
+      </c>
+      <c r="E18" s="5">
+        <v>51864</v>
+      </c>
+      <c r="F18" s="5">
+        <v>86268</v>
+      </c>
+      <c r="G18" s="5">
+        <v>14644</v>
+      </c>
+      <c r="H18" s="95">
+        <v>3992</v>
+      </c>
+      <c r="J18" s="12">
+        <v>31280</v>
+      </c>
+      <c r="K18" s="5">
+        <v>113788</v>
+      </c>
+      <c r="L18" s="5">
+        <v>5552</v>
+      </c>
+      <c r="M18" s="5">
+        <v>52552</v>
+      </c>
+      <c r="N18" s="5">
+        <v>88508</v>
+      </c>
+      <c r="O18" s="5">
+        <v>14796</v>
+      </c>
+      <c r="P18" s="90">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>7387</v>
+      </c>
+      <c r="C19" s="5">
+        <v>10373</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1048</v>
+      </c>
+      <c r="E19" s="5">
+        <v>7159</v>
+      </c>
+      <c r="F19" s="5">
+        <v>14641</v>
+      </c>
+      <c r="G19" s="5">
+        <v>2241</v>
+      </c>
+      <c r="H19" s="95">
+        <v>233</v>
+      </c>
+      <c r="J19" s="12">
+        <v>7411</v>
+      </c>
+      <c r="K19" s="5">
+        <v>10376</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1048</v>
+      </c>
+      <c r="M19" s="5">
+        <v>7329</v>
+      </c>
+      <c r="N19" s="5">
+        <v>15961</v>
+      </c>
+      <c r="O19" s="5">
+        <v>2243</v>
+      </c>
+      <c r="P19" s="90">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5">
+        <v>9</v>
+      </c>
+      <c r="D20" s="91">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="E20" s="5">
+        <v>84</v>
+      </c>
+      <c r="F20" s="5">
+        <v>442</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="95">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>231</v>
+      </c>
+      <c r="K20" s="5">
+        <v>407</v>
+      </c>
+      <c r="L20" s="91">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5">
+        <v>269</v>
+      </c>
+      <c r="N20" s="5">
+        <v>2445</v>
+      </c>
+      <c r="O20" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>31</v>
-      </c>
-      <c r="C14" s="54">
+      <c r="P20" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="80">
+        <v>33</v>
+      </c>
+      <c r="C21" s="80">
+        <v>7</v>
+      </c>
+      <c r="D21" s="92">
+        <v>1</v>
+      </c>
+      <c r="E21" s="80">
+        <v>478</v>
+      </c>
+      <c r="F21" s="80">
+        <v>1503</v>
+      </c>
+      <c r="G21" s="80">
+        <v>6</v>
+      </c>
+      <c r="H21" s="96">
+        <v>1</v>
+      </c>
+      <c r="J21" s="16">
+        <v>32</v>
+      </c>
+      <c r="K21" s="80">
+        <v>2</v>
+      </c>
+      <c r="L21" s="92">
+        <v>1</v>
+      </c>
+      <c r="M21" s="80">
+        <v>538</v>
+      </c>
+      <c r="N21" s="80">
+        <v>1481</v>
+      </c>
+      <c r="O21" s="80">
+        <v>6</v>
+      </c>
+      <c r="P21" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="J22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="3">
-        <v>609</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1885</v>
-      </c>
-      <c r="F14" s="3">
-        <v>6</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="F23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="P23" s="84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="78">
+        <v>11.16226</v>
+      </c>
+      <c r="C24" s="78">
+        <v>19.565930000000002</v>
+      </c>
+      <c r="D24" s="93">
+        <v>1.5231589999999999</v>
+      </c>
+      <c r="E24" s="78">
+        <v>73.041309999999996</v>
+      </c>
+      <c r="F24" s="78">
+        <v>22.832470000000001</v>
+      </c>
+      <c r="G24" s="78">
+        <v>33.381</v>
+      </c>
+      <c r="H24" s="79">
+        <v>2.5567600000000001</v>
+      </c>
+      <c r="J24" s="112">
+        <v>33.811909999999997</v>
+      </c>
+      <c r="K24" s="78">
+        <v>54.367060000000002</v>
+      </c>
+      <c r="L24" s="93">
+        <v>3.0923579999999999</v>
+      </c>
+      <c r="M24" s="78">
+        <v>160.36150000000001</v>
+      </c>
+      <c r="N24" s="78">
+        <v>49.53877</v>
+      </c>
+      <c r="O24" s="78">
+        <v>101.435</v>
+      </c>
+      <c r="P24" s="79">
+        <v>7.2466530000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5">
+        <v>36928</v>
+      </c>
+      <c r="C25" s="5">
+        <v>111332</v>
+      </c>
+      <c r="D25" s="91">
+        <v>2564</v>
+      </c>
+      <c r="E25" s="5">
+        <v>39720</v>
+      </c>
+      <c r="F25" s="5">
+        <v>86208</v>
+      </c>
+      <c r="G25" s="5">
+        <v>31124</v>
+      </c>
+      <c r="H25" s="13">
+        <v>2800</v>
+      </c>
+      <c r="J25" s="12">
+        <v>36444</v>
+      </c>
+      <c r="K25" s="5">
+        <v>111464</v>
+      </c>
+      <c r="L25" s="93">
+        <v>2624</v>
+      </c>
+      <c r="M25" s="5">
+        <v>40356</v>
+      </c>
+      <c r="N25" s="5">
+        <v>85608</v>
+      </c>
+      <c r="O25" s="5">
+        <v>31216</v>
+      </c>
+      <c r="P25" s="13">
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8785</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10577</v>
+      </c>
+      <c r="D26" s="91">
+        <v>306</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4007</v>
+      </c>
+      <c r="F26" s="5">
+        <v>14958</v>
+      </c>
+      <c r="G26" s="5">
+        <v>6872</v>
+      </c>
+      <c r="H26" s="13">
+        <v>436</v>
+      </c>
+      <c r="J26" s="12">
+        <v>8828</v>
+      </c>
+      <c r="K26" s="5">
+        <v>10567</v>
+      </c>
+      <c r="L26" s="93">
+        <v>307</v>
+      </c>
+      <c r="M26" s="5">
+        <v>4244</v>
+      </c>
+      <c r="N26" s="5">
+        <v>15014</v>
+      </c>
+      <c r="O26" s="5">
+        <v>6873</v>
+      </c>
+      <c r="P26" s="13">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C27" s="5">
+        <v>11</v>
+      </c>
+      <c r="D27" s="91">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>79</v>
+      </c>
+      <c r="F27" s="5">
+        <v>404</v>
+      </c>
+      <c r="G27" s="5">
+        <v>18</v>
+      </c>
+      <c r="H27" s="13">
         <v>2</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="J27" s="12">
+        <v>586</v>
+      </c>
+      <c r="K27" s="5">
+        <v>165</v>
+      </c>
+      <c r="L27" s="91">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <v>121</v>
+      </c>
+      <c r="N27" s="5">
+        <v>1788</v>
+      </c>
+      <c r="O27" s="5">
+        <v>24</v>
+      </c>
+      <c r="P27" s="95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="80">
+        <v>23</v>
+      </c>
+      <c r="C28" s="80">
+        <v>9</v>
+      </c>
+      <c r="D28" s="92">
+        <v>1</v>
+      </c>
+      <c r="E28" s="80">
+        <v>317</v>
+      </c>
+      <c r="F28" s="80">
+        <v>1637</v>
+      </c>
+      <c r="G28" s="80">
+        <v>39</v>
+      </c>
+      <c r="H28" s="81">
+        <v>32</v>
+      </c>
+      <c r="J28" s="16">
+        <v>21</v>
+      </c>
+      <c r="K28" s="80">
+        <v>6</v>
+      </c>
+      <c r="L28" s="92">
+        <v>1</v>
+      </c>
+      <c r="M28" s="80">
+        <v>311</v>
+      </c>
+      <c r="N28" s="80">
+        <v>1226</v>
+      </c>
+      <c r="O28" s="80">
+        <v>33</v>
+      </c>
+      <c r="P28" s="81">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="11"/>
+      <c r="J29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="F30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L30" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="M30" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N30" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O30" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="P30" s="84" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="27">
-        <v>11.469049999999999</v>
-      </c>
-      <c r="C17" s="27">
-        <v>11.32404</v>
-      </c>
-      <c r="D17" s="87">
-        <v>5.2743500000000001</v>
-      </c>
-      <c r="E17" s="27">
-        <v>12.21496</v>
-      </c>
-      <c r="F17" s="27">
-        <v>5.6820000000000004</v>
-      </c>
-      <c r="H17" s="27">
-        <v>4.3856599999999997</v>
-      </c>
-      <c r="I17" s="27">
-        <v>9.6299999999999997E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B31" s="78">
+        <v>57.895389999999999</v>
+      </c>
+      <c r="C31" s="78">
+        <v>199.83699999999999</v>
+      </c>
+      <c r="D31" s="78">
+        <v>14.313040000000001</v>
+      </c>
+      <c r="E31" s="78">
+        <v>31.338899999999999</v>
+      </c>
+      <c r="F31" s="78">
+        <v>31.8308</v>
+      </c>
+      <c r="G31" s="78">
+        <v>160.886</v>
+      </c>
+      <c r="H31" s="90">
+        <v>11.158799999999999</v>
+      </c>
+      <c r="J31" s="112">
+        <v>135.65989999999999</v>
+      </c>
+      <c r="K31" s="78">
+        <v>537.95090000000005</v>
+      </c>
+      <c r="L31" s="78">
+        <v>30.123809999999999</v>
+      </c>
+      <c r="M31" s="78">
+        <v>92.060890000000001</v>
+      </c>
+      <c r="N31" s="78">
+        <v>84.975949999999997</v>
+      </c>
+      <c r="O31" s="78">
+        <v>383.13299999999998</v>
+      </c>
+      <c r="P31" s="90">
+        <v>24.383600000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="3">
-        <v>30784</v>
-      </c>
-      <c r="C18" s="3">
-        <v>113672</v>
-      </c>
-      <c r="D18" s="3">
-        <v>52336</v>
-      </c>
-      <c r="E18" s="3">
-        <v>85732</v>
-      </c>
-      <c r="F18" s="54">
-        <v>14832</v>
-      </c>
-      <c r="H18" s="3">
-        <v>5652</v>
-      </c>
-      <c r="I18" s="3">
-        <v>3948</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B32" s="5">
+        <v>29724</v>
+      </c>
+      <c r="C32" s="5">
+        <v>113012</v>
+      </c>
+      <c r="D32" s="91">
+        <v>1740</v>
+      </c>
+      <c r="E32" s="5">
+        <v>51464</v>
+      </c>
+      <c r="F32" s="5">
+        <v>84476</v>
+      </c>
+      <c r="G32" s="5">
+        <v>13748</v>
+      </c>
+      <c r="H32" s="13">
+        <v>3592</v>
+      </c>
+      <c r="J32" s="12">
+        <v>29920</v>
+      </c>
+      <c r="K32" s="5">
+        <v>113492</v>
+      </c>
+      <c r="L32" s="91">
+        <v>1736</v>
+      </c>
+      <c r="M32" s="5">
+        <v>51652</v>
+      </c>
+      <c r="N32" s="5">
+        <v>89188</v>
+      </c>
+      <c r="O32" s="5">
+        <v>13708</v>
+      </c>
+      <c r="P32" s="13">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="3">
-        <v>7340</v>
-      </c>
-      <c r="C19" s="3">
-        <v>10362</v>
-      </c>
-      <c r="D19" s="3">
-        <v>7278</v>
-      </c>
-      <c r="E19" s="3">
-        <v>15846</v>
-      </c>
-      <c r="F19" s="54">
-        <v>2247</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1049</v>
-      </c>
-      <c r="I19" s="3">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B33" s="5">
+        <v>6978</v>
+      </c>
+      <c r="C33" s="5">
+        <v>10298</v>
+      </c>
+      <c r="D33" s="91">
+        <v>73</v>
+      </c>
+      <c r="E33" s="5">
+        <v>7059</v>
+      </c>
+      <c r="F33" s="5">
+        <v>14194</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2048</v>
+      </c>
+      <c r="H33" s="13">
+        <v>137</v>
+      </c>
+      <c r="J33" s="12">
+        <v>6981</v>
+      </c>
+      <c r="K33" s="5">
+        <v>10317</v>
+      </c>
+      <c r="L33" s="91">
+        <v>73</v>
+      </c>
+      <c r="M33" s="5">
+        <v>7105</v>
+      </c>
+      <c r="N33" s="5">
+        <v>15705</v>
+      </c>
+      <c r="O33" s="5">
+        <v>2049</v>
+      </c>
+      <c r="P33" s="13">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B34" s="5">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5">
+        <v>19</v>
+      </c>
+      <c r="D34" s="91">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>133</v>
+      </c>
+      <c r="F34" s="5">
+        <v>774</v>
+      </c>
+      <c r="G34" s="5">
+        <v>4</v>
+      </c>
+      <c r="H34" s="95">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>340</v>
+      </c>
+      <c r="K34" s="5">
+        <v>327</v>
+      </c>
+      <c r="L34" s="91">
+        <v>0</v>
+      </c>
+      <c r="M34" s="5">
+        <v>832</v>
+      </c>
+      <c r="N34" s="5">
+        <v>2480</v>
+      </c>
+      <c r="O34" s="5">
+        <v>14</v>
+      </c>
+      <c r="P34" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="80">
         <v>32</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C35" s="80">
+        <v>23</v>
+      </c>
+      <c r="D35" s="92">
+        <v>1</v>
+      </c>
+      <c r="E35" s="80">
+        <v>531</v>
+      </c>
+      <c r="F35" s="80">
+        <v>1828</v>
+      </c>
+      <c r="G35" s="80">
+        <v>6</v>
+      </c>
+      <c r="H35" s="96">
+        <v>1</v>
+      </c>
+      <c r="J35" s="16">
+        <v>30</v>
+      </c>
+      <c r="K35" s="80">
+        <v>15</v>
+      </c>
+      <c r="L35" s="92">
+        <v>1</v>
+      </c>
+      <c r="M35" s="80">
+        <v>516</v>
+      </c>
+      <c r="N35" s="80">
+        <v>1335</v>
+      </c>
+      <c r="O35" s="80">
+        <v>7</v>
+      </c>
+      <c r="P35" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11"/>
+      <c r="J36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="3">
-        <v>37</v>
-      </c>
-      <c r="E20" s="3">
-        <v>498</v>
-      </c>
-      <c r="F20" s="54">
+      <c r="F37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="3">
+      <c r="K37" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="L37" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N37" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O37" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="78">
+        <v>18.445170000000001</v>
+      </c>
+      <c r="C38" s="78">
+        <v>8.969068</v>
+      </c>
+      <c r="D38" s="93">
+        <v>0.80625400000000003</v>
+      </c>
+      <c r="E38" s="78">
+        <v>23.77093</v>
+      </c>
+      <c r="F38" s="78">
+        <v>6.1581929999999998</v>
+      </c>
+      <c r="G38" s="78">
+        <v>6.4640000000000004</v>
+      </c>
+      <c r="H38" s="79">
+        <v>1.2694099999999999</v>
+      </c>
+      <c r="J38" s="112">
+        <v>61.134169999999997</v>
+      </c>
+      <c r="K38" s="78">
+        <v>17.033930000000002</v>
+      </c>
+      <c r="L38" s="93">
+        <v>1.448099</v>
+      </c>
+      <c r="M38" s="78">
+        <v>95.092439999999996</v>
+      </c>
+      <c r="N38" s="78">
+        <v>11.7454</v>
+      </c>
+      <c r="O38" s="78">
+        <v>16.759</v>
+      </c>
+      <c r="P38" s="79">
+        <v>2.3261699999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="5">
+        <v>32300</v>
+      </c>
+      <c r="C39" s="5">
+        <v>114724</v>
+      </c>
+      <c r="D39" s="91">
+        <v>1708</v>
+      </c>
+      <c r="E39" s="5">
+        <v>54960</v>
+      </c>
+      <c r="F39" s="5">
+        <v>85228</v>
+      </c>
+      <c r="G39" s="5">
+        <v>16480</v>
+      </c>
+      <c r="H39" s="13">
+        <v>3592</v>
+      </c>
+      <c r="J39" s="12">
+        <v>32024</v>
+      </c>
+      <c r="K39" s="5">
+        <v>115588</v>
+      </c>
+      <c r="L39" s="91">
+        <v>1680</v>
+      </c>
+      <c r="M39" s="5">
+        <v>55476</v>
+      </c>
+      <c r="N39" s="5">
+        <v>87004</v>
+      </c>
+      <c r="O39" s="5">
+        <v>16664</v>
+      </c>
+      <c r="P39" s="13">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5">
+        <v>7686</v>
+      </c>
+      <c r="C40" s="5">
+        <v>10673</v>
+      </c>
+      <c r="D40" s="91">
+        <v>81</v>
+      </c>
+      <c r="E40" s="5">
+        <v>8022</v>
+      </c>
+      <c r="F40" s="5">
+        <v>14488</v>
+      </c>
+      <c r="G40" s="5">
+        <v>2673</v>
+      </c>
+      <c r="H40" s="13">
+        <v>146</v>
+      </c>
+      <c r="J40" s="12">
+        <v>7684</v>
+      </c>
+      <c r="K40" s="5">
+        <v>10665</v>
+      </c>
+      <c r="L40" s="91">
+        <v>81</v>
+      </c>
+      <c r="M40" s="5">
+        <v>8140</v>
+      </c>
+      <c r="N40" s="5">
+        <v>16367</v>
+      </c>
+      <c r="O40" s="5">
+        <v>2674</v>
+      </c>
+      <c r="P40" s="13">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="5">
+        <v>12</v>
+      </c>
+      <c r="C41" s="5">
+        <v>13</v>
+      </c>
+      <c r="D41" s="91">
         <v>0</v>
       </c>
-      <c r="I20" s="3">
+      <c r="E41" s="5">
+        <v>225</v>
+      </c>
+      <c r="F41" s="5">
+        <v>664</v>
+      </c>
+      <c r="G41" s="91">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="H41" s="95">
+        <v>0</v>
+      </c>
+      <c r="J41" s="12">
+        <v>412</v>
+      </c>
+      <c r="K41" s="5">
+        <v>4</v>
+      </c>
+      <c r="L41" s="91">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5">
+        <v>712</v>
+      </c>
+      <c r="N41" s="5">
+        <v>3321</v>
+      </c>
+      <c r="O41" s="5">
+        <v>8</v>
+      </c>
+      <c r="P41" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="3">
-        <v>34</v>
-      </c>
-      <c r="C21" s="54">
+      <c r="B42" s="80">
+        <v>50</v>
+      </c>
+      <c r="C42" s="80">
+        <v>18</v>
+      </c>
+      <c r="D42" s="92">
+        <v>1</v>
+      </c>
+      <c r="E42" s="80">
+        <v>519</v>
+      </c>
+      <c r="F42" s="80">
+        <v>1835</v>
+      </c>
+      <c r="G42" s="80">
+        <v>6</v>
+      </c>
+      <c r="H42" s="96">
+        <v>1</v>
+      </c>
+      <c r="J42" s="16">
+        <v>45</v>
+      </c>
+      <c r="K42" s="80">
+        <v>5</v>
+      </c>
+      <c r="L42" s="92">
+        <v>1</v>
+      </c>
+      <c r="M42" s="80">
+        <v>503</v>
+      </c>
+      <c r="N42" s="80">
+        <v>1413</v>
+      </c>
+      <c r="O42" s="80">
+        <v>7</v>
+      </c>
+      <c r="P42" s="81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="11"/>
+      <c r="J43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="3">
-        <v>538</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1579</v>
-      </c>
-      <c r="F21" s="3">
-        <v>7</v>
-      </c>
-      <c r="H21" s="3">
-        <v>1</v>
-      </c>
-      <c r="I21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E44" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="F44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="77"/>
+      <c r="H44" s="87"/>
+      <c r="J44" s="114"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="M44" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N44" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O44" s="115"/>
+      <c r="P44" s="116"/>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="29">
-        <v>35.298760000000001</v>
-      </c>
-      <c r="C24" s="29">
-        <v>0.62096099999999999</v>
-      </c>
-      <c r="D24" s="29">
-        <v>9.8215260000000004</v>
-      </c>
-      <c r="E24" s="29">
-        <v>0.52596299999999996</v>
-      </c>
-      <c r="F24" s="88">
-        <v>6.2E-2</v>
-      </c>
-      <c r="G24" s="29">
-        <v>2.6530000000000001E-2</v>
-      </c>
-      <c r="H24" s="29">
-        <v>5.9064999999999999E-2</v>
-      </c>
-      <c r="I24" s="29"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B45" s="77"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="78">
+        <v>33.734839999999998</v>
+      </c>
+      <c r="E45" s="78">
+        <v>32.516649999999998</v>
+      </c>
+      <c r="F45" s="93">
+        <v>18.341010000000001</v>
+      </c>
+      <c r="G45" s="77"/>
+      <c r="H45" s="87"/>
+      <c r="J45" s="117"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="78">
+        <v>34.077089999999998</v>
+      </c>
+      <c r="M45" s="93">
+        <v>31.280419999999999</v>
+      </c>
+      <c r="N45" s="78">
+        <v>50.343389999999999</v>
+      </c>
+      <c r="O45" s="77"/>
+      <c r="P45" s="87"/>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="3">
-        <v>30908</v>
-      </c>
-      <c r="C25" s="3">
-        <v>110796</v>
-      </c>
-      <c r="D25" s="3">
-        <v>36428</v>
-      </c>
-      <c r="E25" s="3">
-        <v>87592</v>
-      </c>
-      <c r="F25" s="54">
-        <v>12916</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1816</v>
-      </c>
-      <c r="H25" s="3">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="91">
+        <v>32940</v>
+      </c>
+      <c r="E46" s="5">
+        <v>85308</v>
+      </c>
+      <c r="F46" s="5">
+        <v>85616</v>
+      </c>
+      <c r="G46" s="77"/>
+      <c r="H46" s="87"/>
+      <c r="J46" s="117"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="91">
+        <v>32948</v>
+      </c>
+      <c r="M46" s="5">
+        <v>82188</v>
+      </c>
+      <c r="N46" s="5">
+        <v>86016</v>
+      </c>
+      <c r="O46" s="77"/>
+      <c r="P46" s="87"/>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="3">
-        <v>7340</v>
-      </c>
-      <c r="C26" s="3">
-        <v>10330</v>
-      </c>
-      <c r="D26" s="3">
-        <v>3228</v>
-      </c>
-      <c r="E26" s="3">
-        <v>15391</v>
-      </c>
-      <c r="F26" s="54">
-        <v>1805</v>
-      </c>
-      <c r="G26" s="3">
-        <v>189</v>
-      </c>
-      <c r="H26" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="91">
+        <v>7887</v>
+      </c>
+      <c r="E47" s="5">
+        <v>15756</v>
+      </c>
+      <c r="F47" s="5">
+        <v>14919</v>
+      </c>
+      <c r="G47" s="77"/>
+      <c r="H47" s="87"/>
+      <c r="J47" s="117"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="91">
+        <v>7886</v>
+      </c>
+      <c r="M47" s="5">
+        <v>15153</v>
+      </c>
+      <c r="N47" s="5">
+        <v>14612</v>
+      </c>
+      <c r="O47" s="77"/>
+      <c r="P47" s="87"/>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B48" s="77"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="91">
+        <v>60</v>
+      </c>
+      <c r="E48" s="5">
+        <v>201</v>
+      </c>
+      <c r="F48" s="5">
+        <v>576</v>
+      </c>
+      <c r="G48" s="77"/>
+      <c r="H48" s="87"/>
+      <c r="J48" s="117"/>
+      <c r="K48" s="77"/>
+      <c r="L48" s="91">
+        <v>20</v>
+      </c>
+      <c r="M48" s="5">
+        <v>440</v>
+      </c>
+      <c r="N48" s="5">
+        <v>1781</v>
+      </c>
+      <c r="O48" s="77"/>
+      <c r="P48" s="87"/>
+    </row>
+    <row r="49" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="92">
+        <v>1</v>
+      </c>
+      <c r="E49" s="80">
+        <v>582</v>
+      </c>
+      <c r="F49" s="80">
+        <v>1414</v>
+      </c>
+      <c r="G49" s="88"/>
+      <c r="H49" s="89"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="88"/>
+      <c r="L49" s="92">
+        <v>0</v>
+      </c>
+      <c r="M49" s="80">
+        <v>577</v>
+      </c>
+      <c r="N49" s="80">
+        <v>1352</v>
+      </c>
+      <c r="O49" s="88"/>
+      <c r="P49" s="89"/>
+    </row>
+    <row r="50" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="11"/>
+      <c r="J50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="3">
-        <v>3</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="E51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="77"/>
+      <c r="H51" s="87"/>
+      <c r="J51" s="114"/>
+      <c r="K51" s="115"/>
+      <c r="L51" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="M51" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N51" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="O51" s="115"/>
+      <c r="P51" s="116"/>
+    </row>
+    <row r="52" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="3">
-        <v>431</v>
-      </c>
-      <c r="F27" s="54">
-        <v>2</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="B52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="93">
+        <v>1.9934700000000001</v>
+      </c>
+      <c r="E52" s="78">
+        <v>36948.910000000003</v>
+      </c>
+      <c r="F52" s="78">
+        <v>73.519019999999998</v>
+      </c>
+      <c r="G52" s="77"/>
+      <c r="H52" s="87"/>
+      <c r="J52" s="117"/>
+      <c r="K52" s="77"/>
+      <c r="L52" s="93">
+        <v>2.5968870000000002</v>
+      </c>
+      <c r="M52" s="78">
+        <v>64553.98</v>
+      </c>
+      <c r="N52" s="78">
+        <v>127.1751</v>
+      </c>
+      <c r="O52" s="77"/>
+      <c r="P52" s="87"/>
+    </row>
+    <row r="53" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="91">
+        <v>17348</v>
+      </c>
+      <c r="E53" s="5">
+        <v>251496</v>
+      </c>
+      <c r="F53" s="5">
+        <v>86980</v>
+      </c>
+      <c r="G53" s="77"/>
+      <c r="H53" s="87"/>
+      <c r="J53" s="117"/>
+      <c r="K53" s="77"/>
+      <c r="L53" s="91">
+        <v>17236</v>
+      </c>
+      <c r="M53" s="5">
+        <v>642804</v>
+      </c>
+      <c r="N53" s="5">
+        <v>84084</v>
+      </c>
+      <c r="O53" s="77"/>
+      <c r="P53" s="87"/>
+    </row>
+    <row r="54" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="77"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="91">
+        <v>3975</v>
+      </c>
+      <c r="E54" s="5">
+        <v>61097</v>
+      </c>
+      <c r="F54" s="5">
+        <v>15230</v>
+      </c>
+      <c r="G54" s="77"/>
+      <c r="H54" s="87"/>
+      <c r="J54" s="117"/>
+      <c r="K54" s="77"/>
+      <c r="L54" s="91">
+        <v>3975</v>
+      </c>
+      <c r="M54" s="5">
+        <v>159714</v>
+      </c>
+      <c r="N54" s="5">
+        <v>14290</v>
+      </c>
+      <c r="O54" s="77"/>
+      <c r="P54" s="87"/>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="77"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="91">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="E55" s="5">
+        <v>2701</v>
+      </c>
+      <c r="F55" s="5">
+        <v>415</v>
+      </c>
+      <c r="G55" s="77"/>
+      <c r="H55" s="87"/>
+      <c r="J55" s="117"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="91">
+        <v>1</v>
+      </c>
+      <c r="M55" s="5">
+        <v>15956</v>
+      </c>
+      <c r="N55" s="5">
+        <v>2330</v>
+      </c>
+      <c r="O55" s="77"/>
+      <c r="P55" s="87"/>
+    </row>
+    <row r="56" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="3">
-        <v>27</v>
-      </c>
-      <c r="C28" s="54">
-        <v>6</v>
-      </c>
-      <c r="D28" s="3">
-        <v>360</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1701</v>
-      </c>
-      <c r="F28" s="3">
-        <v>7</v>
-      </c>
-      <c r="G28" s="3">
-        <v>16</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="27">
-        <v>107.8066</v>
-      </c>
-      <c r="C31" s="27">
-        <v>369.10899999999998</v>
-      </c>
-      <c r="D31" s="87">
-        <v>53.264330000000001</v>
-      </c>
-      <c r="E31" s="27">
-        <v>57.915089999999999</v>
-      </c>
-      <c r="F31" s="27">
-        <v>318.86599999999999</v>
-      </c>
-      <c r="H31" s="27">
-        <v>25.67023</v>
-      </c>
-      <c r="I31" s="27">
-        <v>923.68799999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="3">
-        <v>29776</v>
-      </c>
-      <c r="C32" s="3">
-        <v>113356</v>
-      </c>
-      <c r="D32" s="3">
-        <v>52848</v>
-      </c>
-      <c r="E32" s="3">
-        <v>86504</v>
-      </c>
-      <c r="F32" s="54">
-        <v>13816</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1648</v>
-      </c>
-      <c r="I32" s="3">
-        <v>3596</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="3">
-        <v>6968</v>
-      </c>
-      <c r="C33" s="3">
-        <v>10320</v>
-      </c>
-      <c r="D33" s="3">
-        <v>7361</v>
-      </c>
-      <c r="E33" s="3">
-        <v>15022</v>
-      </c>
-      <c r="F33" s="54">
-        <v>2050</v>
-      </c>
-      <c r="H33" s="3">
-        <v>72</v>
-      </c>
-      <c r="I33" s="3">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="3">
-        <v>6</v>
-      </c>
-      <c r="C34" s="3">
-        <v>7</v>
-      </c>
-      <c r="D34" s="3">
-        <v>42</v>
-      </c>
-      <c r="E34" s="3">
-        <v>484</v>
-      </c>
-      <c r="F34" s="54">
-        <v>3</v>
-      </c>
-      <c r="H34" s="3">
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="92">
+        <v>1</v>
+      </c>
+      <c r="E56" s="80">
+        <v>6162</v>
+      </c>
+      <c r="F56" s="80">
+        <v>1342</v>
+      </c>
+      <c r="G56" s="88"/>
+      <c r="H56" s="89"/>
+      <c r="J56" s="118"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="92">
         <v>0</v>
       </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="3">
-        <v>32</v>
-      </c>
-      <c r="C35" s="3">
-        <v>14</v>
-      </c>
-      <c r="D35" s="3">
-        <v>624</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1706</v>
-      </c>
-      <c r="F35" s="54">
-        <v>6</v>
-      </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="27">
-        <v>33.263779999999997</v>
-      </c>
-      <c r="C38" s="27">
-        <v>16.30198</v>
-      </c>
-      <c r="D38" s="27">
-        <v>30.977129999999999</v>
-      </c>
-      <c r="E38" s="87">
-        <v>6.0142709999999999</v>
-      </c>
-      <c r="F38" s="27">
-        <v>9.8460000000000001</v>
-      </c>
-      <c r="H38" s="27">
-        <v>1.422339</v>
-      </c>
-      <c r="I38" s="27">
-        <v>0.3468</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="3">
-        <v>32204</v>
-      </c>
-      <c r="C39" s="3">
-        <v>115028</v>
-      </c>
-      <c r="D39" s="3">
-        <v>55840</v>
-      </c>
-      <c r="E39" s="3">
-        <v>88784</v>
-      </c>
-      <c r="F39" s="54">
-        <v>16440</v>
-      </c>
-      <c r="H39" s="3">
-        <v>1772</v>
-      </c>
-      <c r="I39" s="3">
-        <v>3668</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="3">
-        <v>7681</v>
-      </c>
-      <c r="C40" s="3">
-        <v>10692</v>
-      </c>
-      <c r="D40" s="3">
-        <v>8274</v>
-      </c>
-      <c r="E40" s="3">
-        <v>15451</v>
-      </c>
-      <c r="F40" s="54">
-        <v>2675</v>
-      </c>
-      <c r="H40" s="3">
-        <v>83</v>
-      </c>
-      <c r="I40" s="3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="3">
-        <v>4</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1</v>
-      </c>
-      <c r="D41" s="3">
-        <v>47</v>
-      </c>
-      <c r="E41" s="3">
-        <v>545</v>
-      </c>
-      <c r="F41" s="54">
-        <v>0</v>
-      </c>
-      <c r="H41" s="3">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="3">
-        <v>45</v>
-      </c>
-      <c r="C42" s="3">
-        <v>10</v>
-      </c>
-      <c r="D42" s="3">
-        <v>586</v>
-      </c>
-      <c r="E42" s="3">
-        <v>1513</v>
-      </c>
-      <c r="F42" s="54">
-        <v>6</v>
-      </c>
-      <c r="H42" s="3">
-        <v>1</v>
-      </c>
-      <c r="I42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="27">
-        <v>44.744750000000003</v>
-      </c>
-      <c r="E45" s="27">
-        <v>24.17614</v>
-      </c>
-      <c r="H45" s="27">
-        <v>30.8994</v>
-      </c>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="3">
-        <v>73428</v>
-      </c>
-      <c r="E46" s="3">
-        <v>87676</v>
-      </c>
-      <c r="H46" s="3">
-        <v>32884</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="3">
-        <v>12943</v>
-      </c>
-      <c r="E47" s="3">
-        <v>14977</v>
-      </c>
-      <c r="H47" s="3">
-        <v>7886</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="3">
-        <v>73</v>
-      </c>
-      <c r="E48" s="3">
-        <v>455</v>
-      </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="3">
-        <v>572</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1814</v>
-      </c>
-      <c r="H49" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="27">
-        <v>66065.259999999995</v>
-      </c>
-      <c r="E52" s="27">
-        <v>88.230050000000006</v>
-      </c>
-      <c r="H52" s="27">
-        <v>2.3851260000000001</v>
-      </c>
-      <c r="I52" s="27"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="3">
-        <v>714876</v>
-      </c>
-      <c r="E53" s="3">
-        <v>86284</v>
-      </c>
-      <c r="H53" s="3">
-        <v>17296</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="3">
-        <v>175992</v>
-      </c>
-      <c r="E54" s="3">
-        <v>14610</v>
-      </c>
-      <c r="H54" s="3">
-        <v>3975</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="3">
-        <v>613</v>
-      </c>
-      <c r="E55" s="3">
-        <v>372</v>
-      </c>
-      <c r="H55" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="3">
-        <v>3764</v>
-      </c>
-      <c r="E56" s="3">
-        <v>1520</v>
-      </c>
-      <c r="H56" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M56" s="80">
+        <v>4020</v>
+      </c>
+      <c r="N56" s="80">
+        <v>1307</v>
+      </c>
+      <c r="O56" s="88"/>
+      <c r="P56" s="89"/>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9371,72 +10482,1059 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="89"/>
-      <c r="B1" s="89" t="s">
+      <c r="A1" s="77"/>
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="77" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="89">
+      <c r="B2" s="77">
         <v>393</v>
       </c>
-      <c r="C2" s="89">
+      <c r="C2" s="77">
         <v>455</v>
       </c>
-      <c r="D2" s="89">
+      <c r="D2" s="77">
         <v>852</v>
       </c>
-      <c r="E2" s="89">
+      <c r="E2" s="77">
         <v>1242</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="89">
+      <c r="B3" s="77">
         <v>3485</v>
       </c>
-      <c r="C3" s="89">
+      <c r="C3" s="77">
         <v>3212</v>
       </c>
-      <c r="D3" s="89">
+      <c r="D3" s="77">
         <v>4487</v>
       </c>
-      <c r="E3" s="89">
+      <c r="E3" s="77">
         <v>4928</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="89">
+      <c r="B4" s="77">
         <v>1523</v>
       </c>
-      <c r="C4" s="89">
+      <c r="C4" s="77">
         <v>1099</v>
       </c>
-      <c r="D4" s="89">
+      <c r="D4" s="77">
         <v>1550</v>
       </c>
-      <c r="E4" s="89">
+      <c r="E4" s="77">
         <v>2528</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection sqref="A1:F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="98">
+        <v>702.12300000000005</v>
+      </c>
+      <c r="C3" s="78">
+        <v>10.99503</v>
+      </c>
+      <c r="D3" s="78">
+        <v>20.91412</v>
+      </c>
+      <c r="E3" s="78">
+        <v>3.6522019999999999</v>
+      </c>
+      <c r="F3" s="90">
+        <v>2.1619999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>30224</v>
+      </c>
+      <c r="C4" s="99">
+        <v>116836</v>
+      </c>
+      <c r="D4" s="5">
+        <v>54320</v>
+      </c>
+      <c r="E4" s="5">
+        <v>85516</v>
+      </c>
+      <c r="F4" s="95">
+        <v>14016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7320</v>
+      </c>
+      <c r="C5" s="5">
+        <v>11088</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7847</v>
+      </c>
+      <c r="E5" s="99">
+        <v>15231</v>
+      </c>
+      <c r="F5" s="95">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>105</v>
+      </c>
+      <c r="C6" s="5">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5">
+        <v>273</v>
+      </c>
+      <c r="E6" s="99">
+        <v>645</v>
+      </c>
+      <c r="F6" s="95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="80">
+        <v>43</v>
+      </c>
+      <c r="C7" s="80">
+        <v>14</v>
+      </c>
+      <c r="D7" s="80">
+        <v>561</v>
+      </c>
+      <c r="E7" s="100">
+        <v>1479</v>
+      </c>
+      <c r="F7" s="96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="78">
+        <v>2.9347599999999998</v>
+      </c>
+      <c r="C10" s="98">
+        <v>24.868960000000001</v>
+      </c>
+      <c r="D10" s="78">
+        <v>3.7337030000000002</v>
+      </c>
+      <c r="E10" s="78">
+        <v>4.005109</v>
+      </c>
+      <c r="F10" s="90">
+        <v>1.6459999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>29412</v>
+      </c>
+      <c r="C11" s="99">
+        <v>117408</v>
+      </c>
+      <c r="D11" s="5">
+        <v>54152</v>
+      </c>
+      <c r="E11" s="5">
+        <v>85332</v>
+      </c>
+      <c r="F11" s="95">
+        <v>14124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>6943</v>
+      </c>
+      <c r="C12" s="5">
+        <v>11233</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7886</v>
+      </c>
+      <c r="E12" s="99">
+        <v>14574</v>
+      </c>
+      <c r="F12" s="95">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5">
+        <v>400</v>
+      </c>
+      <c r="E13" s="99">
+        <v>637</v>
+      </c>
+      <c r="F13" s="95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="85">
+        <v>43</v>
+      </c>
+      <c r="C14" s="94">
+        <v>6</v>
+      </c>
+      <c r="D14" s="85">
+        <v>542</v>
+      </c>
+      <c r="E14" s="101">
+        <v>1844</v>
+      </c>
+      <c r="F14" s="97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="78">
+        <v>6.0118340000000003</v>
+      </c>
+      <c r="C17" s="78">
+        <v>3.6240809999999999</v>
+      </c>
+      <c r="D17" s="78">
+        <v>3.8552819999999999</v>
+      </c>
+      <c r="E17" s="98">
+        <v>7.5214040000000004</v>
+      </c>
+      <c r="F17" s="93">
+        <v>1.3340000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5">
+        <v>31092</v>
+      </c>
+      <c r="C18" s="99">
+        <v>114132</v>
+      </c>
+      <c r="D18" s="5">
+        <v>51864</v>
+      </c>
+      <c r="E18" s="5">
+        <v>86268</v>
+      </c>
+      <c r="F18" s="91">
+        <v>14644</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>7387</v>
+      </c>
+      <c r="C19" s="5">
+        <v>10373</v>
+      </c>
+      <c r="D19" s="5">
+        <v>7159</v>
+      </c>
+      <c r="E19" s="99">
+        <v>14641</v>
+      </c>
+      <c r="F19" s="91">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5">
+        <v>9</v>
+      </c>
+      <c r="D20" s="5">
+        <v>84</v>
+      </c>
+      <c r="E20" s="99">
+        <v>442</v>
+      </c>
+      <c r="F20" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="80">
+        <v>33</v>
+      </c>
+      <c r="C21" s="80">
+        <v>7</v>
+      </c>
+      <c r="D21" s="80">
+        <v>478</v>
+      </c>
+      <c r="E21" s="100">
+        <v>1503</v>
+      </c>
+      <c r="F21" s="92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="93">
+        <v>11.16226</v>
+      </c>
+      <c r="C24" s="78">
+        <v>19.565930000000002</v>
+      </c>
+      <c r="D24" s="98">
+        <v>73.041309999999996</v>
+      </c>
+      <c r="E24" s="78">
+        <v>22.832470000000001</v>
+      </c>
+      <c r="F24" s="78">
+        <v>33.381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5">
+        <v>36928</v>
+      </c>
+      <c r="C25" s="99">
+        <v>111332</v>
+      </c>
+      <c r="D25" s="5">
+        <v>39720</v>
+      </c>
+      <c r="E25" s="5">
+        <v>86208</v>
+      </c>
+      <c r="F25" s="91">
+        <v>31124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8785</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10577</v>
+      </c>
+      <c r="D26" s="91">
+        <v>4007</v>
+      </c>
+      <c r="E26" s="99">
+        <v>14958</v>
+      </c>
+      <c r="F26" s="5">
+        <v>6872</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5">
+        <v>14</v>
+      </c>
+      <c r="C27" s="91">
+        <v>11</v>
+      </c>
+      <c r="D27" s="5">
+        <v>79</v>
+      </c>
+      <c r="E27" s="99">
+        <v>404</v>
+      </c>
+      <c r="F27" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="80">
+        <v>23</v>
+      </c>
+      <c r="C28" s="92">
+        <v>9</v>
+      </c>
+      <c r="D28" s="80">
+        <v>317</v>
+      </c>
+      <c r="E28" s="100">
+        <v>1637</v>
+      </c>
+      <c r="F28" s="80">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="78">
+        <v>57.895389999999999</v>
+      </c>
+      <c r="C31" s="78">
+        <v>199.83699999999999</v>
+      </c>
+      <c r="D31" s="93">
+        <v>31.338899999999999</v>
+      </c>
+      <c r="E31" s="93">
+        <v>31.8308</v>
+      </c>
+      <c r="F31" s="98">
+        <v>160.886</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5">
+        <v>29724</v>
+      </c>
+      <c r="C32" s="99">
+        <v>113012</v>
+      </c>
+      <c r="D32" s="5">
+        <v>51464</v>
+      </c>
+      <c r="E32" s="5">
+        <v>84476</v>
+      </c>
+      <c r="F32" s="91">
+        <v>13748</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="5">
+        <v>6978</v>
+      </c>
+      <c r="C33" s="5">
+        <v>10298</v>
+      </c>
+      <c r="D33" s="5">
+        <v>7059</v>
+      </c>
+      <c r="E33" s="99">
+        <v>14194</v>
+      </c>
+      <c r="F33" s="91">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5">
+        <v>19</v>
+      </c>
+      <c r="D34" s="5">
+        <v>133</v>
+      </c>
+      <c r="E34" s="99">
+        <v>774</v>
+      </c>
+      <c r="F34" s="91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="80">
+        <v>32</v>
+      </c>
+      <c r="C35" s="80">
+        <v>23</v>
+      </c>
+      <c r="D35" s="80">
+        <v>531</v>
+      </c>
+      <c r="E35" s="100">
+        <v>1828</v>
+      </c>
+      <c r="F35" s="92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="78">
+        <v>18.445170000000001</v>
+      </c>
+      <c r="C38" s="78">
+        <v>8.969068</v>
+      </c>
+      <c r="D38" s="98">
+        <v>23.77093</v>
+      </c>
+      <c r="E38" s="78">
+        <v>6.1581929999999998</v>
+      </c>
+      <c r="F38" s="78">
+        <v>6.4640000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="5">
+        <v>32300</v>
+      </c>
+      <c r="C39" s="99">
+        <v>114724</v>
+      </c>
+      <c r="D39" s="5">
+        <v>54960</v>
+      </c>
+      <c r="E39" s="5">
+        <v>85228</v>
+      </c>
+      <c r="F39" s="5">
+        <v>16480</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5">
+        <v>7686</v>
+      </c>
+      <c r="C40" s="5">
+        <v>10673</v>
+      </c>
+      <c r="D40" s="5">
+        <v>8022</v>
+      </c>
+      <c r="E40" s="99">
+        <v>14488</v>
+      </c>
+      <c r="F40" s="5">
+        <v>2673</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="5">
+        <v>12</v>
+      </c>
+      <c r="C41" s="5">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5">
+        <v>225</v>
+      </c>
+      <c r="E41" s="99">
+        <v>664</v>
+      </c>
+      <c r="F41" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="80">
+        <v>50</v>
+      </c>
+      <c r="C42" s="80">
+        <v>18</v>
+      </c>
+      <c r="D42" s="80">
+        <v>519</v>
+      </c>
+      <c r="E42" s="100">
+        <v>1835</v>
+      </c>
+      <c r="F42" s="80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="77"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="77"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="78">
+        <v>32.516649999999998</v>
+      </c>
+      <c r="E45" s="78">
+        <v>18.341010000000001</v>
+      </c>
+      <c r="F45" s="77"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="5">
+        <v>85308</v>
+      </c>
+      <c r="E46" s="5">
+        <v>85616</v>
+      </c>
+      <c r="F46" s="77"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="5">
+        <v>15756</v>
+      </c>
+      <c r="E47" s="5">
+        <v>14919</v>
+      </c>
+      <c r="F47" s="77"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="77"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="5">
+        <v>201</v>
+      </c>
+      <c r="E48" s="5">
+        <v>576</v>
+      </c>
+      <c r="F48" s="77"/>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="80">
+        <v>582</v>
+      </c>
+      <c r="E49" s="80">
+        <v>1414</v>
+      </c>
+      <c r="F49" s="88"/>
+    </row>
+    <row r="50" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="77"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="78">
+        <v>36948.910000000003</v>
+      </c>
+      <c r="E52" s="78">
+        <v>73.519019999999998</v>
+      </c>
+      <c r="F52" s="77"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="5">
+        <v>251496</v>
+      </c>
+      <c r="E53" s="5">
+        <v>86980</v>
+      </c>
+      <c r="F53" s="77"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="77"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="5">
+        <v>61097</v>
+      </c>
+      <c r="E54" s="5">
+        <v>15230</v>
+      </c>
+      <c r="F54" s="77"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="77"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="5">
+        <v>2701</v>
+      </c>
+      <c r="E55" s="5">
+        <v>415</v>
+      </c>
+      <c r="F55" s="77"/>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="80">
+        <v>6162</v>
+      </c>
+      <c r="E56" s="80">
+        <v>1342</v>
+      </c>
+      <c r="F56" s="88"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>